<commit_message>
Issue with version 1.1
NOT FIXED
</commit_message>
<xml_diff>
--- a/ACCOUNTS.xlsx
+++ b/ACCOUNTS.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtellesy/Documents/GitHub/nadUploader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270E9D52-8072-2B48-969D-CD3949D2EAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA34B4CE-9E8A-3C4F-A8DF-A9A78E8874F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="23960" windowHeight="14380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6180" yWindow="500" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>AC_DESC</t>
   </si>
@@ -50,31 +38,151 @@
     <t>MOBILE_NUMBER</t>
   </si>
   <si>
+    <t>محمد ابوالقاسم</t>
+  </si>
+  <si>
+    <t>LY26002001001201000115924</t>
+  </si>
+  <si>
+    <t>119490021535</t>
+  </si>
+  <si>
+    <t>AC697337</t>
+  </si>
+  <si>
+    <t>0917168698</t>
+  </si>
+  <si>
+    <t>اسماعيل احمد ال</t>
+  </si>
+  <si>
+    <t>LY66002001001201000078926</t>
+  </si>
+  <si>
+    <t>119670326760</t>
+  </si>
+  <si>
+    <t>P1JY8616</t>
+  </si>
+  <si>
+    <t>0910706951</t>
+  </si>
+  <si>
+    <t>صباح مسعود محمد</t>
+  </si>
+  <si>
+    <t>LY61002001001201000093372</t>
+  </si>
+  <si>
+    <t>219570070364</t>
+  </si>
+  <si>
+    <t>AC251547</t>
+  </si>
+  <si>
+    <t>0945547431</t>
+  </si>
+  <si>
+    <t>عمار بشير الصيد</t>
+  </si>
+  <si>
+    <t>LY31002001001201000115058</t>
+  </si>
+  <si>
+    <t>119740495534</t>
+  </si>
+  <si>
+    <t>C07L1G4N</t>
+  </si>
+  <si>
+    <t>0927033581</t>
+  </si>
+  <si>
+    <t>سعدة يونس عبدال</t>
+  </si>
+  <si>
+    <t>LY16002001001201000090496</t>
+  </si>
+  <si>
+    <t>219710471314</t>
+  </si>
+  <si>
+    <t>AA231927</t>
+  </si>
+  <si>
+    <t>0930441990</t>
+  </si>
+  <si>
+    <t>خالد بشير خليفة</t>
+  </si>
+  <si>
+    <t>LY12002001001201000121996</t>
+  </si>
+  <si>
+    <t>119880034318</t>
+  </si>
+  <si>
+    <t>F5KH1PKP</t>
+  </si>
+  <si>
+    <t>0917071553</t>
+  </si>
+  <si>
+    <t>صبحية عمر صاكى</t>
+  </si>
+  <si>
+    <t>LY62002001001201000110620</t>
+  </si>
+  <si>
+    <t>219650297065</t>
+  </si>
+  <si>
+    <t>AD405997</t>
+  </si>
+  <si>
+    <t>0925040190</t>
+  </si>
+  <si>
+    <t>منيرة امحمد محم</t>
+  </si>
+  <si>
+    <t>LY42002001001201000095460</t>
+  </si>
+  <si>
+    <t>219680255536</t>
+  </si>
+  <si>
+    <t>NCN0G4YL</t>
+  </si>
+  <si>
+    <t>0926466942</t>
+  </si>
+  <si>
+    <t>عبد الرحمن سالم</t>
+  </si>
+  <si>
+    <t>LY35002001001201000100630</t>
+  </si>
+  <si>
+    <t>119690113678</t>
+  </si>
+  <si>
+    <t>AD792839</t>
+  </si>
+  <si>
+    <t>0926562522</t>
+  </si>
+  <si>
     <t>Account_no</t>
-  </si>
-  <si>
-    <t>LY26002002021201000115924</t>
-  </si>
-  <si>
-    <t>اسم الزبون</t>
-  </si>
-  <si>
-    <t>119490021000</t>
-  </si>
-  <si>
-    <t>AC690000</t>
-  </si>
-  <si>
-    <t>091245666</t>
-  </si>
-  <si>
-    <t>001201855115924</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="000000000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
@@ -112,11 +220,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,64 +532,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.125" customWidth="1"/>
-    <col min="2" max="2" width="35.875" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.125" customWidth="1"/>
+    <col min="2" max="2" width="28.875" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="16.25" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="28.875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="4">
+        <v>1201000115924</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1201000078926</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1201000093372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1201000115058</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1201000090496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1201000121996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1201000110620</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1201000095460</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1201000100630</v>
+      </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.125" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>